<commit_message>
File Đánh Gía Hoàn Chỉnh
</commit_message>
<xml_diff>
--- a/CS162-KTLT-Summer2020-Project Summary.xlsx
+++ b/CS162-KTLT-Summer2020-Project Summary.xlsx
@@ -644,7 +644,7 @@
     <numFmt numFmtId="166" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="167" formatCode="dd\ mmm\ yy"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -908,6 +908,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1091,7 +1097,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1270,23 +1276,26 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1852,7 +1861,7 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1867,36 +1876,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
@@ -2012,8 +2021,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="97" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2030,33 +2039,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:8" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
@@ -2101,10 +2110,10 @@
       <c r="E7" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="G7" s="67" t="s">
         <v>146</v>
       </c>
       <c r="H7" s="3">
@@ -2119,17 +2128,17 @@
       <c r="D8" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="66" t="s">
         <v>144</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>147</v>
       </c>
       <c r="H8" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2140,13 +2149,13 @@
       <c r="D9" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="67" t="s">
         <v>148</v>
       </c>
       <c r="H9" s="3">
@@ -2188,7 +2197,7 @@
       <c r="E14" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="65" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2260,11 +2269,11 @@
   <dimension ref="A1:BP81"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="11" ySplit="6" topLeftCell="Q29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="6" topLeftCell="L53" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2311,28 +2320,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:68" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
     </row>
     <row r="2" spans="1:68" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2370,15 +2379,15 @@
       </c>
     </row>
     <row r="3" spans="1:68" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
       <c r="AW3" s="2"/>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
@@ -2849,7 +2858,7 @@
       </c>
       <c r="E8" s="32">
         <f>SUM(E9:E13)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
@@ -2867,9 +2876,11 @@
       <c r="D9" s="38">
         <v>1</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="38">
+        <v>1</v>
+      </c>
       <c r="F9" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="33">
         <v>2</v>
@@ -2895,21 +2906,23 @@
       <c r="D10" s="38">
         <v>1</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="38">
+        <v>1</v>
+      </c>
       <c r="F10" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G10" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="34">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2923,21 +2936,23 @@
       <c r="D11" s="38">
         <v>1</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="38">
+        <v>1</v>
+      </c>
       <c r="F11" s="33">
+        <v>1</v>
+      </c>
+      <c r="G11" s="33">
         <v>3</v>
       </c>
-      <c r="G11" s="33">
+      <c r="H11" s="33">
         <v>2</v>
-      </c>
-      <c r="H11" s="33">
-        <v>3</v>
       </c>
       <c r="I11" s="33">
         <v>2</v>
       </c>
       <c r="J11" s="34">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2951,18 +2966,23 @@
       <c r="D12" s="38">
         <v>1</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="38">
+        <v>1</v>
+      </c>
       <c r="F12" s="33">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G12" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="33">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I12" s="33">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="J12" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:68" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2976,11 +2996,24 @@
       <c r="D13" s="38">
         <v>1</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
+      <c r="E13" s="38">
+        <v>1</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="G13" s="33">
+        <v>2</v>
+      </c>
+      <c r="H13" s="33">
+        <v>2</v>
+      </c>
+      <c r="I13" s="33">
+        <v>2</v>
+      </c>
+      <c r="J13" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
@@ -2996,14 +3029,14 @@
       </c>
       <c r="E14" s="32">
         <f>SUM(E15:E21)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
     </row>
-    <row r="15" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>2.1</v>
       </c>
@@ -3014,13 +3047,26 @@
       <c r="D15" s="38">
         <v>3</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="38">
+        <v>3</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
+      <c r="G15" s="68">
+        <v>4</v>
+      </c>
+      <c r="H15" s="68">
+        <v>6</v>
+      </c>
+      <c r="I15" s="68">
+        <v>3</v>
+      </c>
+      <c r="J15" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>2.2000000000000002</v>
       </c>
@@ -3031,13 +3077,26 @@
       <c r="D16" s="38">
         <v>1</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="38">
+        <v>1</v>
+      </c>
+      <c r="F16" s="68">
+        <v>5</v>
+      </c>
+      <c r="G16" s="68">
+        <v>4</v>
+      </c>
+      <c r="H16" s="68">
+        <v>7</v>
+      </c>
+      <c r="I16" s="68">
+        <v>2</v>
+      </c>
+      <c r="J16" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>2.2999999999999998</v>
       </c>
@@ -3048,13 +3107,26 @@
       <c r="D17" s="38">
         <v>1</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="38">
+        <v>1</v>
+      </c>
+      <c r="F17" s="68">
+        <v>5</v>
+      </c>
+      <c r="G17" s="68">
+        <v>4</v>
+      </c>
+      <c r="H17" s="68">
+        <v>7</v>
+      </c>
+      <c r="I17" s="68">
+        <v>2</v>
+      </c>
+      <c r="J17" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>2.4</v>
       </c>
@@ -3065,13 +3137,26 @@
       <c r="D18" s="38">
         <v>1</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="38">
+        <v>1</v>
+      </c>
+      <c r="F18" s="68">
+        <v>5</v>
+      </c>
+      <c r="G18" s="68">
+        <v>4</v>
+      </c>
+      <c r="H18" s="68">
+        <v>7</v>
+      </c>
+      <c r="I18" s="68">
+        <v>2</v>
+      </c>
+      <c r="J18" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>2.5</v>
       </c>
@@ -3082,13 +3167,26 @@
       <c r="D19" s="38">
         <v>1</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="38">
+        <v>1</v>
+      </c>
+      <c r="F19" s="68">
+        <v>5</v>
+      </c>
+      <c r="G19" s="68">
+        <v>4</v>
+      </c>
+      <c r="H19" s="68">
+        <v>7</v>
+      </c>
+      <c r="I19" s="68">
+        <v>2</v>
+      </c>
+      <c r="J19" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>2.6</v>
       </c>
@@ -3099,13 +3197,26 @@
       <c r="D20" s="38">
         <v>1</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="38">
+        <v>1</v>
+      </c>
+      <c r="F20" s="68">
+        <v>5</v>
+      </c>
+      <c r="G20" s="68">
+        <v>4</v>
+      </c>
+      <c r="H20" s="68">
+        <v>7</v>
+      </c>
+      <c r="I20" s="68">
+        <v>2</v>
+      </c>
+      <c r="J20" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>2.7</v>
       </c>
@@ -3116,13 +3227,26 @@
       <c r="D21" s="38">
         <v>1</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="38">
+        <v>1</v>
+      </c>
+      <c r="F21" s="68">
+        <v>5</v>
+      </c>
+      <c r="G21" s="68">
+        <v>4</v>
+      </c>
+      <c r="H21" s="68">
+        <v>7</v>
+      </c>
+      <c r="I21" s="68">
+        <v>2</v>
+      </c>
+      <c r="J21" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>3</v>
       </c>
@@ -3135,14 +3259,14 @@
       </c>
       <c r="E22" s="41">
         <f>SUM(E23:E33)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>3.1</v>
       </c>
@@ -3153,13 +3277,26 @@
       <c r="D23" s="38">
         <v>1</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="38">
+        <v>1</v>
+      </c>
+      <c r="F23" s="68">
+        <v>10</v>
+      </c>
+      <c r="G23" s="68">
+        <v>3</v>
+      </c>
+      <c r="H23" s="68">
+        <v>12</v>
+      </c>
+      <c r="I23" s="68">
+        <v>5</v>
+      </c>
+      <c r="J23" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>3.2</v>
       </c>
@@ -3170,13 +3307,26 @@
       <c r="D24" s="38">
         <v>3</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="38">
+        <v>3</v>
+      </c>
+      <c r="F24" s="68">
+        <v>10</v>
+      </c>
+      <c r="G24" s="68">
+        <v>3</v>
+      </c>
+      <c r="H24" s="68">
+        <v>14</v>
+      </c>
+      <c r="I24" s="68">
+        <v>5</v>
+      </c>
+      <c r="J24" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>3.3</v>
       </c>
@@ -3187,13 +3337,26 @@
       <c r="D25" s="38">
         <v>1</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-    </row>
-    <row r="26" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="38">
+        <v>1</v>
+      </c>
+      <c r="F25" s="68">
+        <v>10</v>
+      </c>
+      <c r="G25" s="68">
+        <v>3</v>
+      </c>
+      <c r="H25" s="68">
+        <v>14</v>
+      </c>
+      <c r="I25" s="68">
+        <v>3</v>
+      </c>
+      <c r="J25" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>3.4</v>
       </c>
@@ -3204,13 +3367,26 @@
       <c r="D26" s="38">
         <v>1</v>
       </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="38">
+        <v>1</v>
+      </c>
+      <c r="F26" s="68">
+        <v>10</v>
+      </c>
+      <c r="G26" s="68">
+        <v>3</v>
+      </c>
+      <c r="H26" s="68">
+        <v>14</v>
+      </c>
+      <c r="I26" s="68">
+        <v>3</v>
+      </c>
+      <c r="J26" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>3.5</v>
       </c>
@@ -3221,13 +3397,26 @@
       <c r="D27" s="38">
         <v>1</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="38">
+        <v>1</v>
+      </c>
+      <c r="F27" s="68">
+        <v>10</v>
+      </c>
+      <c r="G27" s="68">
+        <v>3</v>
+      </c>
+      <c r="H27" s="68">
+        <v>14</v>
+      </c>
+      <c r="I27" s="68">
+        <v>5</v>
+      </c>
+      <c r="J27" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>3.6</v>
       </c>
@@ -3238,13 +3427,26 @@
       <c r="D28" s="38">
         <v>1</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="38">
+        <v>1</v>
+      </c>
+      <c r="F28" s="68">
+        <v>10</v>
+      </c>
+      <c r="G28" s="68">
+        <v>3</v>
+      </c>
+      <c r="H28" s="68">
+        <v>14</v>
+      </c>
+      <c r="I28" s="68">
+        <v>6</v>
+      </c>
+      <c r="J28" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>3.7</v>
       </c>
@@ -3255,13 +3457,26 @@
       <c r="D29" s="38">
         <v>1</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="38">
+        <v>1</v>
+      </c>
+      <c r="F29" s="68">
+        <v>10</v>
+      </c>
+      <c r="G29" s="68">
+        <v>3</v>
+      </c>
+      <c r="H29" s="68">
+        <v>14</v>
+      </c>
+      <c r="I29" s="68">
+        <v>5</v>
+      </c>
+      <c r="J29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>3.8</v>
       </c>
@@ -3272,13 +3487,26 @@
       <c r="D30" s="38">
         <v>1</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="38">
+        <v>1</v>
+      </c>
+      <c r="F30" s="68">
+        <v>10</v>
+      </c>
+      <c r="G30" s="68">
+        <v>3</v>
+      </c>
+      <c r="H30" s="68">
+        <v>14</v>
+      </c>
+      <c r="I30" s="68">
+        <v>4</v>
+      </c>
+      <c r="J30" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>3.9</v>
       </c>
@@ -3289,13 +3517,26 @@
       <c r="D31" s="38">
         <v>1</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-    </row>
-    <row r="32" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="38">
+        <v>1</v>
+      </c>
+      <c r="F31" s="68">
+        <v>10</v>
+      </c>
+      <c r="G31" s="68">
+        <v>3</v>
+      </c>
+      <c r="H31" s="68">
+        <v>14</v>
+      </c>
+      <c r="I31" s="68">
+        <v>5</v>
+      </c>
+      <c r="J31" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="35">
         <v>3.1</v>
       </c>
@@ -3306,13 +3547,26 @@
       <c r="D32" s="38">
         <v>1</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="38">
+        <v>1</v>
+      </c>
+      <c r="F32" s="68">
+        <v>10</v>
+      </c>
+      <c r="G32" s="68">
+        <v>3</v>
+      </c>
+      <c r="H32" s="68">
+        <v>14</v>
+      </c>
+      <c r="I32" s="68">
+        <v>6</v>
+      </c>
+      <c r="J32" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>3.11</v>
       </c>
@@ -3323,13 +3577,26 @@
       <c r="D33" s="38">
         <v>1</v>
       </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="38">
+        <v>1</v>
+      </c>
+      <c r="F33" s="68">
+        <v>10</v>
+      </c>
+      <c r="G33" s="68">
+        <v>3</v>
+      </c>
+      <c r="H33" s="68">
+        <v>14</v>
+      </c>
+      <c r="I33" s="68">
+        <v>5</v>
+      </c>
+      <c r="J33" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>4</v>
       </c>
@@ -3342,14 +3609,14 @@
       </c>
       <c r="E34" s="41">
         <f>SUM(E35:E39)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>4.0999999999999996</v>
       </c>
@@ -3360,13 +3627,26 @@
       <c r="D35" s="38">
         <v>1</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-    </row>
-    <row r="36" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="38">
+        <v>1</v>
+      </c>
+      <c r="F35" s="68">
+        <v>19</v>
+      </c>
+      <c r="G35" s="68">
+        <v>5</v>
+      </c>
+      <c r="H35" s="68">
+        <v>28</v>
+      </c>
+      <c r="I35" s="68">
+        <v>2</v>
+      </c>
+      <c r="J35" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="35">
         <v>4.2</v>
       </c>
@@ -3377,13 +3657,26 @@
       <c r="D36" s="38">
         <v>1</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-    </row>
-    <row r="37" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="38">
+        <v>1</v>
+      </c>
+      <c r="F36" s="68">
+        <v>19</v>
+      </c>
+      <c r="G36" s="68">
+        <v>5</v>
+      </c>
+      <c r="H36" s="68">
+        <v>19</v>
+      </c>
+      <c r="I36" s="68">
+        <v>1</v>
+      </c>
+      <c r="J36" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>5</v>
       </c>
@@ -3398,7 +3691,7 @@
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>5.0999999999999996</v>
       </c>
@@ -3409,13 +3702,26 @@
       <c r="D38" s="38">
         <v>1</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-    </row>
-    <row r="39" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="68">
+        <v>19</v>
+      </c>
+      <c r="G38" s="68">
+        <v>5</v>
+      </c>
+      <c r="H38" s="68">
+        <v>28</v>
+      </c>
+      <c r="I38" s="68">
+        <v>3</v>
+      </c>
+      <c r="J38" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>5.2</v>
       </c>
@@ -3426,13 +3732,26 @@
       <c r="D39" s="38">
         <v>1</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-    </row>
-    <row r="40" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="38">
+        <v>1</v>
+      </c>
+      <c r="F39" s="68">
+        <v>19</v>
+      </c>
+      <c r="G39" s="68">
+        <v>5</v>
+      </c>
+      <c r="H39" s="68">
+        <v>20</v>
+      </c>
+      <c r="I39" s="68">
+        <v>2</v>
+      </c>
+      <c r="J39" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>6</v>
       </c>
@@ -3445,14 +3764,14 @@
       </c>
       <c r="E40" s="41">
         <f>SUM(E41:E47)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
       <c r="H40" s="33"/>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>6.1</v>
       </c>
@@ -3463,13 +3782,26 @@
       <c r="D41" s="38">
         <v>1</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-    </row>
-    <row r="42" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E41" s="38">
+        <v>1</v>
+      </c>
+      <c r="F41" s="68">
+        <v>19</v>
+      </c>
+      <c r="G41" s="68">
+        <v>5</v>
+      </c>
+      <c r="H41" s="68">
+        <v>28</v>
+      </c>
+      <c r="I41" s="68">
+        <v>3</v>
+      </c>
+      <c r="J41" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>6.2</v>
       </c>
@@ -3480,13 +3812,26 @@
       <c r="D42" s="38">
         <v>1</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-    </row>
-    <row r="43" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E42" s="38">
+        <v>1</v>
+      </c>
+      <c r="F42" s="68">
+        <v>19</v>
+      </c>
+      <c r="G42" s="68">
+        <v>5</v>
+      </c>
+      <c r="H42" s="68">
+        <v>28</v>
+      </c>
+      <c r="I42" s="68">
+        <v>3</v>
+      </c>
+      <c r="J42" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>6.3</v>
       </c>
@@ -3497,13 +3842,26 @@
       <c r="D43" s="38">
         <v>1</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-    </row>
-    <row r="44" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E43" s="38">
+        <v>1</v>
+      </c>
+      <c r="F43" s="68">
+        <v>19</v>
+      </c>
+      <c r="G43" s="68">
+        <v>5</v>
+      </c>
+      <c r="H43" s="68">
+        <v>28</v>
+      </c>
+      <c r="I43" s="68">
+        <v>2</v>
+      </c>
+      <c r="J43" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>6.4</v>
       </c>
@@ -3514,13 +3872,26 @@
       <c r="D44" s="38">
         <v>1</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-    </row>
-    <row r="45" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E44" s="38">
+        <v>1</v>
+      </c>
+      <c r="F44" s="68">
+        <v>19</v>
+      </c>
+      <c r="G44" s="68">
+        <v>5</v>
+      </c>
+      <c r="H44" s="68">
+        <v>22</v>
+      </c>
+      <c r="I44" s="68">
+        <v>4</v>
+      </c>
+      <c r="J44" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>6.5</v>
       </c>
@@ -3531,13 +3902,26 @@
       <c r="D45" s="38">
         <v>2</v>
       </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E45" s="38">
+        <v>2</v>
+      </c>
+      <c r="F45" s="68">
+        <v>19</v>
+      </c>
+      <c r="G45" s="68">
+        <v>5</v>
+      </c>
+      <c r="H45" s="68">
+        <v>19</v>
+      </c>
+      <c r="I45" s="68">
+        <v>1</v>
+      </c>
+      <c r="J45" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>6.6</v>
       </c>
@@ -3548,13 +3932,26 @@
       <c r="D46" s="38">
         <v>1</v>
       </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-    </row>
-    <row r="47" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="38">
+        <v>1</v>
+      </c>
+      <c r="F46" s="68">
+        <v>19</v>
+      </c>
+      <c r="G46" s="68">
+        <v>5</v>
+      </c>
+      <c r="H46" s="68">
+        <v>27</v>
+      </c>
+      <c r="I46" s="68">
+        <v>1</v>
+      </c>
+      <c r="J46" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>6.7</v>
       </c>
@@ -3565,13 +3962,26 @@
       <c r="D47" s="38">
         <v>1</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-    </row>
-    <row r="48" spans="1:9" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="38">
+        <v>1</v>
+      </c>
+      <c r="F47" s="68">
+        <v>19</v>
+      </c>
+      <c r="G47" s="68">
+        <v>5</v>
+      </c>
+      <c r="H47" s="68">
+        <v>28</v>
+      </c>
+      <c r="I47" s="68">
+        <v>2</v>
+      </c>
+      <c r="J47" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>7</v>
       </c>
@@ -3584,14 +3994,17 @@
       </c>
       <c r="E48" s="41">
         <f>SUM(E49:E52)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
       <c r="H48" s="33"/>
       <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>7.1</v>
       </c>
@@ -3602,13 +4015,26 @@
       <c r="D49" s="38">
         <v>3</v>
       </c>
-      <c r="E49" s="38"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-    </row>
-    <row r="50" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E49" s="38">
+        <v>3</v>
+      </c>
+      <c r="F49" s="68">
+        <v>19</v>
+      </c>
+      <c r="G49" s="68">
+        <v>10</v>
+      </c>
+      <c r="H49" s="68">
+        <v>21</v>
+      </c>
+      <c r="I49" s="68">
+        <v>2</v>
+      </c>
+      <c r="J49" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35">
         <v>7.2</v>
       </c>
@@ -3619,13 +4045,26 @@
       <c r="D50" s="38">
         <v>1</v>
       </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-    </row>
-    <row r="51" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E50" s="38">
+        <v>1</v>
+      </c>
+      <c r="F50" s="68">
+        <v>19</v>
+      </c>
+      <c r="G50" s="68">
+        <v>10</v>
+      </c>
+      <c r="H50" s="68">
+        <v>28</v>
+      </c>
+      <c r="I50" s="68">
+        <v>2</v>
+      </c>
+      <c r="J50" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>7.3</v>
       </c>
@@ -3636,13 +4075,26 @@
       <c r="D51" s="38">
         <v>1</v>
       </c>
-      <c r="E51" s="38"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-    </row>
-    <row r="52" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="38">
+        <v>1</v>
+      </c>
+      <c r="F51" s="68">
+        <v>19</v>
+      </c>
+      <c r="G51" s="68">
+        <v>10</v>
+      </c>
+      <c r="H51" s="68">
+        <v>28</v>
+      </c>
+      <c r="I51" s="68">
+        <v>4</v>
+      </c>
+      <c r="J51" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35">
         <v>7.4</v>
       </c>
@@ -3653,16 +4105,29 @@
       <c r="D52" s="38">
         <v>1</v>
       </c>
-      <c r="E52" s="38"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E52" s="38">
+        <v>1</v>
+      </c>
+      <c r="F52" s="68">
+        <v>19</v>
+      </c>
+      <c r="G52" s="68">
+        <v>10</v>
+      </c>
+      <c r="H52" s="68">
+        <v>25</v>
+      </c>
+      <c r="I52" s="68">
+        <v>1</v>
+      </c>
+      <c r="J52" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="42"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="42"/>
       <c r="B54" s="43" t="s">
         <v>101</v>
@@ -3674,41 +4139,41 @@
       </c>
       <c r="E54" s="43">
         <f>SUM(E8,E14,E22,E34,E40,E48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="42"/>
       <c r="B55" s="40" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="40" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="40" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" s="40" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" s="40" t="s">
         <v>134</v>
       </c>

</xml_diff>